<commit_message>
edit POM + src code to dynamic
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestJAVA\JAVA\CucumberCRM\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DDCA14-7CED-4E39-BDB7-752025F2C4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918D2DC-ACD6-4006-ADEB-961944AAD0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{087FA7D4-EF6F-413D-ABC6-FDC0D1BECD89}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>EMAIL</t>
   </si>
@@ -43,9 +43,6 @@
     <t>nameCompany</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>languageDefault</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>groups</t>
   </si>
   <si>
-    <t>Thanh_19062023</t>
-  </si>
-  <si>
     <t>EUR</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>Thanh_20062023</t>
-  </si>
-  <si>
     <t>nameProject</t>
   </si>
   <si>
@@ -98,6 +89,18 @@
   </si>
   <si>
     <t>Thanh Project 02</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Thanh_06092023</t>
+  </si>
+  <si>
+    <t>Thanh_07092023</t>
+  </si>
+  <si>
+    <t>VIP</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,33 +530,33 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +570,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,33 +586,33 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +625,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,24 +639,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>70</v>
@@ -672,7 +675,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,18 +688,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>

</xml_diff>